<commit_message>
cleaning up this directory with commits
</commit_message>
<xml_diff>
--- a/subjectsUnique_List.xlsx
+++ b/subjectsUnique_List.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/davie.yoon/Dropbox/hcp7tret-cmf/dyoon_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{981FB607-1DC7-7643-BC93-98753A180FB1}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44619BD-CC25-9344-B0F6-D44B9D8FCCA0}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15940" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -561,10 +561,10 @@
     <t>Ventral stripes swirled together</t>
   </si>
   <si>
-    <t>DY final adjust 10/20/2018</t>
-  </si>
-  <si>
     <t>Slight LH d V2/V3 stripes</t>
+  </si>
+  <si>
+    <t>DY final adjust - mostly for Y branches 10/20/2018</t>
   </si>
 </sst>
 </file>
@@ -3324,8 +3324,8 @@
   <dimension ref="A1:M182"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E121" sqref="E121"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3341,7 +3341,7 @@
     <col min="12" max="12" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="51" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="85" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -3379,7 +3379,7 @@
         <v>23</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -7845,7 +7845,7 @@
         <v>9</v>
       </c>
       <c r="L125" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="M125" s="12">
         <v>43394</v>

</xml_diff>